<commit_message>
Initial commit - Portal de Fretes ready for Render deployment
</commit_message>
<xml_diff>
--- a/Lojas Portal.xlsx
+++ b/Lojas Portal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/61bfe54e086fb976/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/61bfe54e086fb976/Desktop/Portal de Fretes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75DBE4DC-8B8E-47BE-8F9D-7ECACB880C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{75DBE4DC-8B8E-47BE-8F9D-7ECACB880C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35E666A3-86BF-4DDF-B9A5-CCEC086DC272}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9024,6 +9024,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9345,7 +9349,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K872"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E64" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -39884,7 +39890,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K872" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>